<commit_message>
renew r code, plots, and data
</commit_message>
<xml_diff>
--- a/result/tw_tour_risk.xlsx
+++ b/result/tw_tour_risk.xlsx
@@ -380,12 +380,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>cn_psg_dense</t>
+          <t>risk</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ln_twexpose</t>
+          <t>ln_tw_risk</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -524,10 +524,10 @@
         <v>185</v>
       </c>
       <c r="E2">
-        <v>86828.1781021901</v>
+        <v>0.00614137489401504</v>
       </c>
       <c r="F2">
-        <v>16.59205382249096</v>
+        <v>5.22647841858601</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="E4">
-        <v>178744.7075518089</v>
+        <v>0.0127563015870867</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -797,10 +797,10 @@
         <v>6698</v>
       </c>
       <c r="E5">
-        <v>3037815.47405249</v>
+        <v>0.209665059032301</v>
       </c>
       <c r="F5">
-        <v>23.73621380354627</v>
+        <v>8.999907763926535</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="E6">
-        <v>370176.6547961765</v>
+        <v>0.0227748818358775</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -981,10 +981,10 @@
         <v>113</v>
       </c>
       <c r="E7">
-        <v>8582394.02694848</v>
+        <v>0.168347664564615</v>
       </c>
       <c r="F7">
-        <v>20.69261139189396</v>
+        <v>4.882978316844667</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1076,10 +1076,10 @@
         <v>16</v>
       </c>
       <c r="E8">
-        <v>224715.3847457626</v>
+        <v>0.0256975843456798</v>
       </c>
       <c r="F8">
-        <v>15.09518309607149</v>
+        <v>2.797961673440694</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1171,10 +1171,10 @@
         <v>24</v>
       </c>
       <c r="E9">
-        <v>23890.7396875</v>
+        <v>0.00272292284457534</v>
       </c>
       <c r="F9">
-        <v>13.2593418887574</v>
+        <v>3.18077305275393</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1266,10 +1266,10 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>229952.424328023</v>
+        <v>0.0364116937993349</v>
       </c>
       <c r="F10">
-        <v>14.54285664181343</v>
+        <v>2.232989030073072</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1361,10 +1361,10 @@
         <v>1131</v>
       </c>
       <c r="E11">
-        <v>8410721.792727094</v>
+        <v>0.288755608721611</v>
       </c>
       <c r="F11">
-        <v>22.97587544881066</v>
+        <v>7.284534584519009</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1456,10 +1456,10 @@
         <v>55</v>
       </c>
       <c r="E12">
-        <v>323572.7499999992</v>
+        <v>0.0186017066066913</v>
       </c>
       <c r="F12">
-        <v>16.69451552744363</v>
+        <v>4.025763996142878</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1551,10 +1551,10 @@
         <v>427</v>
       </c>
       <c r="E13">
-        <v>3995987.863247867</v>
+        <v>0.214874128821924</v>
       </c>
       <c r="F13">
-        <v>21.25758564500032</v>
+        <v>6.251424486977098</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1646,10 +1646,10 @@
         <v>11897</v>
       </c>
       <c r="E14">
-        <v>55759390.28362726</v>
+        <v>1.7381126844623</v>
       </c>
       <c r="F14">
-        <v>27.22059795411231</v>
+        <v>10.39131042825277</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1741,10 +1741,10 @@
         <v>230</v>
       </c>
       <c r="E15">
-        <v>3616672.969040243</v>
+        <v>0.193823271504487</v>
       </c>
       <c r="F15">
-        <v>20.53914467729326</v>
+        <v>5.615240299123142</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1836,10 +1836,10 @@
         <v>52</v>
       </c>
       <c r="E16">
-        <v>139837.1020862902</v>
+        <v>0.0583578599868634</v>
       </c>
       <c r="F16">
-        <v>15.79948433734129</v>
+        <v>4.007962236780179</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1931,10 +1931,10 @@
         <v>2463</v>
       </c>
       <c r="E17">
-        <v>5686806.459410318</v>
+        <v>0.425575082414661</v>
       </c>
       <c r="F17">
-        <v>23.36279496756947</v>
+        <v>8.16371069703683</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2026,10 +2026,10 @@
         <v>3259</v>
       </c>
       <c r="E18">
-        <v>9897151.416182896</v>
+        <v>0.782980903505756</v>
       </c>
       <c r="F18">
-        <v>24.19693331783858</v>
+        <v>8.667462307344751</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2121,10 +2121,10 @@
         <v>13</v>
       </c>
       <c r="E19">
-        <v>27529.81145617667</v>
+        <v>0.00670371765539473</v>
       </c>
       <c r="F19">
-        <v>12.78801043050622</v>
+        <v>2.571630705120837</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2216,10 +2216,10 @@
         <v>561</v>
       </c>
       <c r="E20">
-        <v>341294.4156164654</v>
+        <v>0.13908364323229</v>
       </c>
       <c r="F20">
-        <v>19.07022460820442</v>
+        <v>6.459945022965127</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2311,10 +2311,10 @@
         <v>10924</v>
       </c>
       <c r="E21">
-        <v>16865081.88302302</v>
+        <v>1.02003057516788</v>
       </c>
       <c r="F21">
-        <v>25.93947342355825</v>
+        <v>10.00183013011388</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2403,7 +2403,7 @@
         </is>
       </c>
       <c r="E22">
-        <v>104.2199094834678</v>
+        <v>2.21977405807772e-05</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2495,10 +2495,10 @@
         <v>11528</v>
       </c>
       <c r="E23">
-        <v>52418653.00046701</v>
+        <v>1.4112805513978</v>
       </c>
       <c r="F23">
-        <v>27.1273072159957</v>
+        <v>10.23269209319368</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2587,7 +2587,7 @@
         </is>
       </c>
       <c r="E24">
-        <v>260513.3314671614</v>
+        <v>0.029530394219294</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -2676,7 +2676,7 @@
         </is>
       </c>
       <c r="E25">
-        <v>40461.60000000001</v>
+        <v>8.8790962323109e-05</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -2768,10 +2768,10 @@
         <v>216</v>
       </c>
       <c r="E26">
-        <v>1631204.754072924</v>
+        <v>0.145025238461078</v>
       </c>
       <c r="F26">
-        <v>19.68010843342947</v>
+        <v>5.510705086771525</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -2952,10 +2952,10 @@
         <v>73</v>
       </c>
       <c r="E28">
-        <v>163985.232308792</v>
+        <v>0.0166039099544214</v>
       </c>
       <c r="F28">
-        <v>16.29799719509415</v>
+        <v>4.306927013280672</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -3047,10 +3047,10 @@
         <v>301</v>
       </c>
       <c r="E29">
-        <v>1385089.188777199</v>
+        <v>0.0949767326982856</v>
       </c>
       <c r="F29">
-        <v>19.84838607848303</v>
+        <v>5.797843379114219</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -3142,10 +3142,10 @@
         <v>146</v>
       </c>
       <c r="E30">
-        <v>489366.4200319352</v>
+        <v>0.0513951686913596</v>
       </c>
       <c r="F30">
-        <v>18.08447547823652</v>
+        <v>5.033724635981492</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -3237,10 +3237,10 @@
         <v>285</v>
       </c>
       <c r="E31">
-        <v>18798.49795511221</v>
+        <v>0.0394379857651809</v>
       </c>
       <c r="F31">
-        <v>15.49407462421481</v>
+        <v>5.691169349051433</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -3332,10 +3332,10 @@
         <v>1689</v>
       </c>
       <c r="E32">
-        <v>11746403.39186692</v>
+        <v>0.211714650412593</v>
       </c>
       <c r="F32">
-        <v>23.71094965932906</v>
+        <v>7.623928339781987</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -3427,10 +3427,10 @@
         <v>6926</v>
       </c>
       <c r="E33">
-        <v>31417939.2769633</v>
+        <v>1.13150762836454</v>
       </c>
       <c r="F33">
-        <v>26.10592735908474</v>
+        <v>9.599867261050562</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -3522,10 +3522,10 @@
         <v>88</v>
       </c>
       <c r="E34">
-        <v>4281414.992668624</v>
+        <v>0.0473181836713568</v>
       </c>
       <c r="F34">
-        <v>19.74713116672945</v>
+        <v>4.523569600552934</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -3795,10 +3795,10 @@
         <v>38</v>
       </c>
       <c r="E37">
-        <v>56421.22219600747</v>
+        <v>0.00937484577194826</v>
       </c>
       <c r="F37">
-        <v>14.57820453017826</v>
+        <v>3.646917334359665</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -3890,10 +3890,10 @@
         <v>26</v>
       </c>
       <c r="E38">
-        <v>492934.9333333336</v>
+        <v>0.0145839155615707</v>
       </c>
       <c r="F38">
-        <v>16.36623102993101</v>
+        <v>3.272575131061424</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -3985,10 +3985,10 @@
         <v>6</v>
       </c>
       <c r="E39">
-        <v>32904.2715342554</v>
+        <v>0.00785800016559514</v>
       </c>
       <c r="F39">
-        <v>12.19314762215095</v>
+        <v>1.799586756102128</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -4080,10 +4080,10 @@
         <v>719</v>
       </c>
       <c r="E40">
-        <v>1370285.880376428</v>
+        <v>0.125594816206038</v>
       </c>
       <c r="F40">
-        <v>20.70839203533849</v>
+        <v>6.696172979167821</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -4261,7 +4261,7 @@
         </is>
       </c>
       <c r="E42">
-        <v>53113.51551886321</v>
+        <v>0.00318167614991141</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -4353,10 +4353,10 @@
         <v>6</v>
       </c>
       <c r="E43">
-        <v>76479.7425852498</v>
+        <v>0.00685170259259991</v>
       </c>
       <c r="F43">
-        <v>13.03655372644137</v>
+        <v>1.79858780557809</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -4448,10 +4448,10 @@
         <v>36</v>
       </c>
       <c r="E44">
-        <v>2225749.03125</v>
+        <v>0.0108990906251616</v>
       </c>
       <c r="F44">
-        <v>18.19912344793224</v>
+        <v>3.59435906206405</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -4531,7 +4531,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>蒙特內哥羅</t>
+          <t xml:space="preserve">蒙特內哥羅</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -4540,7 +4540,7 @@
         </is>
       </c>
       <c r="E45">
-        <v>35860.02788104088</v>
+        <v>0.00573441631670079</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -4632,10 +4632,10 @@
         <v>9121</v>
       </c>
       <c r="E46">
-        <v>22944513.31662214</v>
+        <v>0.331937613398083</v>
       </c>
       <c r="F46">
-        <v>26.06692416448117</v>
+        <v>9.404969460413254</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -4727,10 +4727,10 @@
         <v>654</v>
       </c>
       <c r="E47">
-        <v>108725.2489451063</v>
+        <v>0.0552723740461353</v>
       </c>
       <c r="F47">
-        <v>18.0796958760505</v>
+        <v>6.536906259515253</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -4822,10 +4822,10 @@
         <v>437</v>
       </c>
       <c r="E48">
-        <v>2129820.202188184</v>
+        <v>0.127052467837509</v>
       </c>
       <c r="F48">
-        <v>20.65148178662316</v>
+        <v>6.199538984382349</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -4917,10 +4917,10 @@
         <v>1063</v>
       </c>
       <c r="E49">
-        <v>2099214.498961433</v>
+        <v>0.138388114027426</v>
       </c>
       <c r="F49">
-        <v>21.5259246393171</v>
+        <v>7.098463705135256</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -5101,10 +5101,10 @@
         <v>39</v>
       </c>
       <c r="E51">
-        <v>469835.7907510429</v>
+        <v>0.0410732193212982</v>
       </c>
       <c r="F51">
-        <v>16.72370230578817</v>
+        <v>3.703813768852255</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -5196,10 +5196,10 @@
         <v>463</v>
       </c>
       <c r="E52">
-        <v>1334542.440506031</v>
+        <v>1.11930627029197</v>
       </c>
       <c r="F52">
-        <v>20.24182685327976</v>
+        <v>6.888815858224056</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -5377,7 +5377,7 @@
         </is>
       </c>
       <c r="E54">
-        <v>810212.3315344153</v>
+        <v>0.0750949563847694</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -5469,10 +5469,10 @@
         <v>5</v>
       </c>
       <c r="E55">
-        <v>13141.70707154742</v>
+        <v>0.0008583126357900529</v>
       </c>
       <c r="F55">
-        <v>11.09306020087556</v>
+        <v>1.610295856930237</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -5564,10 +5564,10 @@
         <v>55</v>
       </c>
       <c r="E56">
-        <v>103460.9783794091</v>
+        <v>0.00745844083514115</v>
       </c>
       <c r="F56">
-        <v>15.55429265077426</v>
+        <v>4.014763949428953</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -5659,10 +5659,10 @@
         <v>1244</v>
       </c>
       <c r="E57">
-        <v>502870.9875770294</v>
+        <v>0.148828451347251</v>
       </c>
       <c r="F57">
-        <v>20.25417819213214</v>
+        <v>7.264829958449162</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -5751,7 +5751,7 @@
         </is>
       </c>
       <c r="E58">
-        <v>1473.073724336982</v>
+        <v>0.000118387949764145</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -5843,10 +5843,10 @@
         <v>130</v>
       </c>
       <c r="E59">
-        <v>216773.1336766222</v>
+        <v>0.0215466068570744</v>
       </c>
       <c r="F59">
-        <v>17.15414568227558</v>
+        <v>4.888852210590512</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -5938,10 +5938,10 @@
         <v>10068</v>
       </c>
       <c r="E60">
-        <v>7111778.970102485</v>
+        <v>0.491975923738626</v>
       </c>
       <c r="F60">
-        <v>24.99438047411539</v>
+        <v>9.617218721002168</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -6033,10 +6033,10 @@
         <v>13</v>
       </c>
       <c r="E61">
-        <v>1330687.503495658</v>
+        <v>0.127821989510976</v>
       </c>
       <c r="F61">
-        <v>16.6661563955149</v>
+        <v>2.685237687366762</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -6213,6 +6213,9 @@
           <t>Vatican</t>
         </is>
       </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
       <c r="G63">
         <v>0</v>
       </c>
@@ -6299,6 +6302,9 @@
           <t>Jersey</t>
         </is>
       </c>
+      <c r="E64">
+        <v>8.8790962323109e-05</v>
+      </c>
       <c r="G64">
         <v>0</v>
       </c>
@@ -6384,6 +6390,9 @@
         <is>
           <t>Guernsey</t>
         </is>
+      </c>
+      <c r="E65">
+        <v>0</v>
       </c>
       <c r="G65">
         <v>0</v>

</xml_diff>